<commit_message>
bo ci ejecucion 2
</commit_message>
<xml_diff>
--- a/output/ejecucion_2/gridsearch_results/base0/b0_ci_results_gs_rf_nrs.xlsx
+++ b/output/ejecucion_2/gridsearch_results/base0/b0_ci_results_gs_rf_nrs.xlsx
@@ -561,16 +561,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>146.9704323291779</v>
+        <v>117.24279961586</v>
       </c>
       <c r="C2">
-        <v>32.55125489703917</v>
+        <v>2.174562564397549</v>
       </c>
       <c r="D2">
-        <v>6.111600637435913</v>
+        <v>4.316183614730835</v>
       </c>
       <c r="E2">
-        <v>1.512889062353626</v>
+        <v>0.8705940045061311</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -585,28 +585,28 @@
         <v>16</v>
       </c>
       <c r="J2">
-        <v>0.8282828282828283</v>
+        <v>0.8</v>
       </c>
       <c r="K2">
-        <v>0.8585858585858586</v>
+        <v>0.7957446808510639</v>
       </c>
       <c r="L2">
-        <v>0.8344594594594594</v>
+        <v>0.8595744680851064</v>
       </c>
       <c r="M2">
-        <v>0.8581081081081081</v>
+        <v>0.7872340425531915</v>
       </c>
       <c r="N2">
-        <v>0.8614864864864865</v>
+        <v>0.8376068376068376</v>
       </c>
       <c r="O2">
-        <v>0.8481845481845482</v>
+        <v>0.8160320058192398</v>
       </c>
       <c r="P2">
-        <v>0.01391447000620245</v>
+        <v>0.02778252270785624</v>
       </c>
       <c r="Q2">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -614,16 +614,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>326.4535569667816</v>
+        <v>256.1425208568573</v>
       </c>
       <c r="C3">
-        <v>2.125791300186585</v>
+        <v>2.401137283086126</v>
       </c>
       <c r="D3">
-        <v>7.791748952865601</v>
+        <v>7.226261520385743</v>
       </c>
       <c r="E3">
-        <v>1.052261314170407</v>
+        <v>0.6399036488235725</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -638,28 +638,28 @@
         <v>17</v>
       </c>
       <c r="J3">
-        <v>0.8282828282828283</v>
+        <v>0.8</v>
       </c>
       <c r="K3">
-        <v>0.8653198653198653</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="L3">
-        <v>0.8378378378378378</v>
+        <v>0.8553191489361702</v>
       </c>
       <c r="M3">
-        <v>0.8581081081081081</v>
+        <v>0.7957446808510639</v>
       </c>
       <c r="N3">
-        <v>0.8581081081081081</v>
+        <v>0.8418803418803419</v>
       </c>
       <c r="O3">
-        <v>0.8495313495313495</v>
+        <v>0.8194398981633025</v>
       </c>
       <c r="P3">
-        <v>0.01403308004072782</v>
+        <v>0.02433449631349397</v>
       </c>
       <c r="Q3">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -667,16 +667,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>662.5653190612793</v>
+        <v>513.606924533844</v>
       </c>
       <c r="C4">
-        <v>5.46574680178702</v>
+        <v>2.117344906592611</v>
       </c>
       <c r="D4">
-        <v>7.659553337097168</v>
+        <v>6.704575061798096</v>
       </c>
       <c r="E4">
-        <v>0.7352229619410603</v>
+        <v>0.1638492561984789</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -691,25 +691,25 @@
         <v>18</v>
       </c>
       <c r="J4">
-        <v>0.835016835016835</v>
+        <v>0.8085106382978723</v>
       </c>
       <c r="K4">
-        <v>0.8619528619528619</v>
+        <v>0.8</v>
       </c>
       <c r="L4">
-        <v>0.8378378378378378</v>
+        <v>0.8595744680851064</v>
       </c>
       <c r="M4">
-        <v>0.8547297297297297</v>
+        <v>0.8</v>
       </c>
       <c r="N4">
-        <v>0.8547297297297297</v>
+        <v>0.8376068376068376</v>
       </c>
       <c r="O4">
-        <v>0.8488533988533987</v>
+        <v>0.8211383887979633</v>
       </c>
       <c r="P4">
-        <v>0.01052094621145159</v>
+        <v>0.02367135417240987</v>
       </c>
       <c r="Q4">
         <v>22</v>
@@ -720,16 +720,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>253.2948615074158</v>
+        <v>198.5927383422851</v>
       </c>
       <c r="C5">
-        <v>5.192956063782757</v>
+        <v>3.575088612362944</v>
       </c>
       <c r="D5">
-        <v>8.405112504959106</v>
+        <v>7.973670291900635</v>
       </c>
       <c r="E5">
-        <v>1.039134764665363</v>
+        <v>0.9700928078182841</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -744,28 +744,28 @@
         <v>19</v>
       </c>
       <c r="J5">
-        <v>0.8215488215488216</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="K5">
-        <v>0.8585858585858586</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="L5">
-        <v>0.8412162162162162</v>
+        <v>0.8595744680851064</v>
       </c>
       <c r="M5">
-        <v>0.847972972972973</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="N5">
-        <v>0.8581081081081081</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O5">
-        <v>0.8454863954863955</v>
+        <v>0.8279614475359155</v>
       </c>
       <c r="P5">
-        <v>0.01362592020828197</v>
+        <v>0.02432294122911954</v>
       </c>
       <c r="Q5">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -773,16 +773,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>480.3610237598419</v>
+        <v>383.6331405639648</v>
       </c>
       <c r="C6">
-        <v>1.713620848036373</v>
+        <v>3.800772794723251</v>
       </c>
       <c r="D6">
-        <v>6.800271892547608</v>
+        <v>7.991287565231323</v>
       </c>
       <c r="E6">
-        <v>1.443951007759892</v>
+        <v>1.044054203521473</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -797,25 +797,25 @@
         <v>20</v>
       </c>
       <c r="J6">
-        <v>0.8282828282828283</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="K6">
-        <v>0.8653198653198653</v>
+        <v>0.8</v>
       </c>
       <c r="L6">
-        <v>0.8445945945945946</v>
+        <v>0.8595744680851064</v>
       </c>
       <c r="M6">
-        <v>0.847972972972973</v>
+        <v>0.8</v>
       </c>
       <c r="N6">
-        <v>0.8581081081081081</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="O6">
-        <v>0.8488556738556738</v>
+        <v>0.8219967266775777</v>
       </c>
       <c r="P6">
-        <v>0.0126400559527784</v>
+        <v>0.02560516581018469</v>
       </c>
       <c r="Q6">
         <v>21</v>
@@ -826,16 +826,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>964.6007441043854</v>
+        <v>765.5123206138611</v>
       </c>
       <c r="C7">
-        <v>6.128753880918515</v>
+        <v>3.506681120777958</v>
       </c>
       <c r="D7">
-        <v>9.459297943115235</v>
+        <v>7.201497554779053</v>
       </c>
       <c r="E7">
-        <v>0.3942369427722919</v>
+        <v>1.713151653163561</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -850,28 +850,28 @@
         <v>21</v>
       </c>
       <c r="J7">
-        <v>0.8282828282828283</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="K7">
-        <v>0.8686868686868687</v>
+        <v>0.8085106382978723</v>
       </c>
       <c r="L7">
-        <v>0.8513513513513513</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M7">
-        <v>0.8547297297297297</v>
+        <v>0.8</v>
       </c>
       <c r="N7">
-        <v>0.8581081081081081</v>
+        <v>0.8418803418803419</v>
       </c>
       <c r="O7">
-        <v>0.8522317772317771</v>
+        <v>0.8236952173122385</v>
       </c>
       <c r="P7">
-        <v>0.01331066017548234</v>
+        <v>0.02494564836713176</v>
       </c>
       <c r="Q7">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -879,16 +879,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>330.7063404083252</v>
+        <v>263.5560977935791</v>
       </c>
       <c r="C8">
-        <v>4.65807373507984</v>
+        <v>2.055202132737892</v>
       </c>
       <c r="D8">
-        <v>7.363575744628906</v>
+        <v>6.801190662384033</v>
       </c>
       <c r="E8">
-        <v>0.7055262513056623</v>
+        <v>2.110451185550037</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -903,28 +903,28 @@
         <v>22</v>
       </c>
       <c r="J8">
-        <v>0.8215488215488216</v>
+        <v>0.7957446808510639</v>
       </c>
       <c r="K8">
-        <v>0.8552188552188552</v>
+        <v>0.7957446808510639</v>
       </c>
       <c r="L8">
-        <v>0.8378378378378378</v>
+        <v>0.8595744680851064</v>
       </c>
       <c r="M8">
-        <v>0.8513513513513513</v>
+        <v>0.8</v>
       </c>
       <c r="N8">
-        <v>0.8581081081081081</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="O8">
-        <v>0.8448129948129948</v>
+        <v>0.8168794326241133</v>
       </c>
       <c r="P8">
-        <v>0.01354744733912905</v>
+        <v>0.02558072560461545</v>
       </c>
       <c r="Q8">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -932,16 +932,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>649.9629706859589</v>
+        <v>511.3886632442474</v>
       </c>
       <c r="C9">
-        <v>4.246501144158734</v>
+        <v>3.529579199041532</v>
       </c>
       <c r="D9">
-        <v>8.617614984512329</v>
+        <v>6.569707536697388</v>
       </c>
       <c r="E9">
-        <v>0.6450504633704252</v>
+        <v>1.438428939823716</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -956,28 +956,28 @@
         <v>23</v>
       </c>
       <c r="J9">
-        <v>0.8282828282828283</v>
+        <v>0.7872340425531915</v>
       </c>
       <c r="K9">
-        <v>0.8619528619528619</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="L9">
-        <v>0.831081081081081</v>
+        <v>0.8595744680851064</v>
       </c>
       <c r="M9">
-        <v>0.8547297297297297</v>
+        <v>0.7829787234042553</v>
       </c>
       <c r="N9">
-        <v>0.8581081081081081</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="O9">
-        <v>0.8468309218309219</v>
+        <v>0.8160392798690671</v>
       </c>
       <c r="P9">
-        <v>0.01421498102368304</v>
+        <v>0.03118911199879478</v>
       </c>
       <c r="Q9">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -985,16 +985,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1297.101744270325</v>
+        <v>987.6739552021027</v>
       </c>
       <c r="C10">
-        <v>8.186677520162474</v>
+        <v>5.423287140432095</v>
       </c>
       <c r="D10">
-        <v>8.600317430496215</v>
+        <v>9.539885377883911</v>
       </c>
       <c r="E10">
-        <v>1.113370159119707</v>
+        <v>0.2945026170023527</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -1009,25 +1009,25 @@
         <v>24</v>
       </c>
       <c r="J10">
-        <v>0.8249158249158249</v>
+        <v>0.7957446808510639</v>
       </c>
       <c r="K10">
-        <v>0.8653198653198653</v>
+        <v>0.8</v>
       </c>
       <c r="L10">
-        <v>0.831081081081081</v>
+        <v>0.8553191489361702</v>
       </c>
       <c r="M10">
-        <v>0.8547297297297297</v>
+        <v>0.7872340425531915</v>
       </c>
       <c r="N10">
-        <v>0.8614864864864865</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="O10">
-        <v>0.8475065975065975</v>
+        <v>0.8168903436988544</v>
       </c>
       <c r="P10">
-        <v>0.01640160992880264</v>
+        <v>0.02808930263670127</v>
       </c>
       <c r="Q10">
         <v>24</v>
@@ -1038,16 +1038,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>241.8832600593567</v>
+        <v>177.9753852367401</v>
       </c>
       <c r="C11">
-        <v>5.385905901324003</v>
+        <v>2.04019547916774</v>
       </c>
       <c r="D11">
-        <v>7.925419616699219</v>
+        <v>6.86268835067749</v>
       </c>
       <c r="E11">
-        <v>0.5185562347671437</v>
+        <v>0.751223112367547</v>
       </c>
       <c r="F11">
         <v>20</v>
@@ -1062,28 +1062,28 @@
         <v>25</v>
       </c>
       <c r="J11">
-        <v>0.8484848484848485</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="K11">
-        <v>0.8686868686868687</v>
+        <v>0.7914893617021277</v>
       </c>
       <c r="L11">
-        <v>0.8648648648648649</v>
+        <v>0.8553191489361702</v>
       </c>
       <c r="M11">
-        <v>0.847972972972973</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="N11">
-        <v>0.8547297297297297</v>
+        <v>0.8504273504273504</v>
       </c>
       <c r="O11">
-        <v>0.8569478569478569</v>
+        <v>0.8237024913620659</v>
       </c>
       <c r="P11">
-        <v>0.008456648909940636</v>
+        <v>0.02519661877532901</v>
       </c>
       <c r="Q11">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1091,16 +1091,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>464.2232013225556</v>
+        <v>344.9748812675476</v>
       </c>
       <c r="C12">
-        <v>16.14714407328842</v>
+        <v>5.019945002688534</v>
       </c>
       <c r="D12">
-        <v>8.801383686065673</v>
+        <v>8.6109769821167</v>
       </c>
       <c r="E12">
-        <v>0.5619913276121363</v>
+        <v>0.5647154518595646</v>
       </c>
       <c r="F12">
         <v>20</v>
@@ -1115,28 +1115,28 @@
         <v>26</v>
       </c>
       <c r="J12">
-        <v>0.8417508417508418</v>
+        <v>0.8212765957446808</v>
       </c>
       <c r="K12">
-        <v>0.8686868686868687</v>
+        <v>0.8</v>
       </c>
       <c r="L12">
-        <v>0.8648648648648649</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M12">
-        <v>0.8547297297297297</v>
+        <v>0.8127659574468085</v>
       </c>
       <c r="N12">
-        <v>0.8614864864864865</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O12">
-        <v>0.8583037583037584</v>
+        <v>0.8305146390252773</v>
       </c>
       <c r="P12">
-        <v>0.009463187474365854</v>
+        <v>0.02460232698404185</v>
       </c>
       <c r="Q12">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1144,16 +1144,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>909.5973459720611</v>
+        <v>687.115966463089</v>
       </c>
       <c r="C13">
-        <v>20.95941140803293</v>
+        <v>13.08317948563759</v>
       </c>
       <c r="D13">
-        <v>8.34173812866211</v>
+        <v>8.804060697555542</v>
       </c>
       <c r="E13">
-        <v>1.086044440208922</v>
+        <v>1.083229573095264</v>
       </c>
       <c r="F13">
         <v>20</v>
@@ -1168,28 +1168,28 @@
         <v>27</v>
       </c>
       <c r="J13">
-        <v>0.8383838383838383</v>
+        <v>0.8212765957446808</v>
       </c>
       <c r="K13">
-        <v>0.8720538720538721</v>
+        <v>0.8</v>
       </c>
       <c r="L13">
-        <v>0.875</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M13">
-        <v>0.8547297297297297</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="N13">
-        <v>0.8581081081081081</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O13">
-        <v>0.8596551096551096</v>
+        <v>0.8288125113657028</v>
       </c>
       <c r="P13">
-        <v>0.01317812225933154</v>
+        <v>0.02602469002656995</v>
       </c>
       <c r="Q13">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1197,16 +1197,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>347.9623205184936</v>
+        <v>262.7763268947601</v>
       </c>
       <c r="C14">
-        <v>10.14105533324011</v>
+        <v>5.664971772453887</v>
       </c>
       <c r="D14">
-        <v>8.243627166748047</v>
+        <v>8.17674412727356</v>
       </c>
       <c r="E14">
-        <v>0.8083711841229181</v>
+        <v>1.074615604430521</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -1221,28 +1221,28 @@
         <v>28</v>
       </c>
       <c r="J14">
-        <v>0.835016835016835</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="K14">
-        <v>0.8653198653198653</v>
+        <v>0.7957446808510639</v>
       </c>
       <c r="L14">
-        <v>0.8682432432432432</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M14">
-        <v>0.8513513513513513</v>
+        <v>0.8212765957446808</v>
       </c>
       <c r="N14">
-        <v>0.8682432432432432</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="O14">
-        <v>0.8576349076349077</v>
+        <v>0.8288052373158756</v>
       </c>
       <c r="P14">
-        <v>0.01292433698030795</v>
+        <v>0.02373282913395365</v>
       </c>
       <c r="Q14">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1250,16 +1250,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>675.9000642776489</v>
+        <v>507.0535025119781</v>
       </c>
       <c r="C15">
-        <v>14.79463048166024</v>
+        <v>12.34151562123702</v>
       </c>
       <c r="D15">
-        <v>7.986394500732422</v>
+        <v>8.09945363998413</v>
       </c>
       <c r="E15">
-        <v>0.4954761450238968</v>
+        <v>0.636005628188543</v>
       </c>
       <c r="F15">
         <v>20</v>
@@ -1274,28 +1274,28 @@
         <v>29</v>
       </c>
       <c r="J15">
-        <v>0.8383838383838383</v>
+        <v>0.8297872340425532</v>
       </c>
       <c r="K15">
-        <v>0.8686868686868687</v>
+        <v>0.8</v>
       </c>
       <c r="L15">
-        <v>0.8682432432432432</v>
+        <v>0.8680851063829788</v>
       </c>
       <c r="M15">
-        <v>0.8547297297297297</v>
+        <v>0.8127659574468085</v>
       </c>
       <c r="N15">
-        <v>0.8716216216216216</v>
+        <v>0.8376068376068376</v>
       </c>
       <c r="O15">
-        <v>0.8603330603330605</v>
+        <v>0.8296490270958354</v>
       </c>
       <c r="P15">
-        <v>0.01243345793958175</v>
+        <v>0.02325846464735015</v>
       </c>
       <c r="Q15">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1303,16 +1303,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1343.862488174439</v>
+        <v>1011.812148523331</v>
       </c>
       <c r="C16">
-        <v>35.89544944404924</v>
+        <v>28.37094455592142</v>
       </c>
       <c r="D16">
-        <v>9.331275272369385</v>
+        <v>8.216314983367919</v>
       </c>
       <c r="E16">
-        <v>0.4995011120628026</v>
+        <v>1.029025306480224</v>
       </c>
       <c r="F16">
         <v>20</v>
@@ -1327,28 +1327,28 @@
         <v>30</v>
       </c>
       <c r="J16">
-        <v>0.8316498316498316</v>
+        <v>0.8340425531914893</v>
       </c>
       <c r="K16">
-        <v>0.8754208754208754</v>
+        <v>0.7957446808510639</v>
       </c>
       <c r="L16">
-        <v>0.8682432432432432</v>
+        <v>0.8680851063829788</v>
       </c>
       <c r="M16">
-        <v>0.8547297297297297</v>
+        <v>0.825531914893617</v>
       </c>
       <c r="N16">
-        <v>0.8648648648648649</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="O16">
-        <v>0.8589817089817091</v>
+        <v>0.833911620294599</v>
       </c>
       <c r="P16">
-        <v>0.01520358233629005</v>
+        <v>0.02385225824922545</v>
       </c>
       <c r="Q16">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1356,16 +1356,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>451.3470545768738</v>
+        <v>342.7055951595306</v>
       </c>
       <c r="C17">
-        <v>16.66429669703903</v>
+        <v>4.982647272542039</v>
       </c>
       <c r="D17">
-        <v>8.503309154510498</v>
+        <v>8.478762865066528</v>
       </c>
       <c r="E17">
-        <v>0.6459831508770014</v>
+        <v>0.6277816854955187</v>
       </c>
       <c r="F17">
         <v>20</v>
@@ -1380,28 +1380,28 @@
         <v>31</v>
       </c>
       <c r="J17">
-        <v>0.8249158249158249</v>
+        <v>0.8212765957446808</v>
       </c>
       <c r="K17">
-        <v>0.8585858585858586</v>
+        <v>0.8</v>
       </c>
       <c r="L17">
-        <v>0.8682432432432432</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M17">
-        <v>0.8547297297297297</v>
+        <v>0.8297872340425532</v>
       </c>
       <c r="N17">
-        <v>0.8716216216216216</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O17">
-        <v>0.8556192556192557</v>
+        <v>0.8339188943444261</v>
       </c>
       <c r="P17">
-        <v>0.01653924682465459</v>
+        <v>0.02303884161147782</v>
       </c>
       <c r="Q17">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1409,16 +1409,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>884.5518761157989</v>
+        <v>669.3677783966065</v>
       </c>
       <c r="C18">
-        <v>25.11998494386114</v>
+        <v>17.90084138637779</v>
       </c>
       <c r="D18">
-        <v>9.129681539535522</v>
+        <v>8.534052848815918</v>
       </c>
       <c r="E18">
-        <v>0.1397405853035606</v>
+        <v>0.5106648354242365</v>
       </c>
       <c r="F18">
         <v>20</v>
@@ -1433,28 +1433,28 @@
         <v>32</v>
       </c>
       <c r="J18">
-        <v>0.8282828282828283</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="K18">
-        <v>0.8720538720538721</v>
+        <v>0.8127659574468085</v>
       </c>
       <c r="L18">
-        <v>0.8682432432432432</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M18">
-        <v>0.8547297297297297</v>
+        <v>0.8212765957446808</v>
       </c>
       <c r="N18">
-        <v>0.8682432432432432</v>
+        <v>0.8504273504273504</v>
       </c>
       <c r="O18">
-        <v>0.8583105833105833</v>
+        <v>0.8330641934897255</v>
       </c>
       <c r="P18">
-        <v>0.01612874475296526</v>
+        <v>0.02027975348371419</v>
       </c>
       <c r="Q18">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1462,16 +1462,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1753.16418671608</v>
+        <v>1294.169502973557</v>
       </c>
       <c r="C19">
-        <v>46.7399129626483</v>
+        <v>33.01858457252234</v>
       </c>
       <c r="D19">
-        <v>8.779425525665284</v>
+        <v>9.183200407028199</v>
       </c>
       <c r="E19">
-        <v>1.088341311640476</v>
+        <v>0.4723768765713295</v>
       </c>
       <c r="F19">
         <v>20</v>
@@ -1486,28 +1486,28 @@
         <v>33</v>
       </c>
       <c r="J19">
-        <v>0.835016835016835</v>
+        <v>0.8297872340425532</v>
       </c>
       <c r="K19">
-        <v>0.8686868686868687</v>
+        <v>0.8085106382978723</v>
       </c>
       <c r="L19">
-        <v>0.8682432432432432</v>
+        <v>0.8553191489361702</v>
       </c>
       <c r="M19">
-        <v>0.8581081081081081</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="N19">
-        <v>0.8716216216216216</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O19">
-        <v>0.8603353353353353</v>
+        <v>0.8330678305146388</v>
       </c>
       <c r="P19">
-        <v>0.01345845737398862</v>
+        <v>0.01915420999359483</v>
       </c>
       <c r="Q19">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1515,16 +1515,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>249.5852912425995</v>
+        <v>179.8314328193665</v>
       </c>
       <c r="C20">
-        <v>7.747057687937973</v>
+        <v>7.298643056738277</v>
       </c>
       <c r="D20">
-        <v>8.970130681991577</v>
+        <v>9.10414423942566</v>
       </c>
       <c r="E20">
-        <v>0.2100231614411422</v>
+        <v>0.6032023512399088</v>
       </c>
       <c r="F20">
         <v>30</v>
@@ -1539,28 +1539,28 @@
         <v>34</v>
       </c>
       <c r="J20">
-        <v>0.8451178451178452</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="K20">
-        <v>0.8653198653198653</v>
+        <v>0.7914893617021277</v>
       </c>
       <c r="L20">
-        <v>0.8716216216216216</v>
+        <v>0.8595744680851064</v>
       </c>
       <c r="M20">
-        <v>0.847972972972973</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="N20">
-        <v>0.8547297297297297</v>
+        <v>0.8589743589743589</v>
       </c>
       <c r="O20">
-        <v>0.8569524069524069</v>
+        <v>0.8288161483906163</v>
       </c>
       <c r="P20">
-        <v>0.01010769608749628</v>
+        <v>0.02655981514184416</v>
       </c>
       <c r="Q20">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1568,16 +1568,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>488.4824663162232</v>
+        <v>354.7139088630676</v>
       </c>
       <c r="C21">
-        <v>16.30741772768682</v>
+        <v>7.923010173600854</v>
       </c>
       <c r="D21">
-        <v>8.680505180358887</v>
+        <v>8.440692138671874</v>
       </c>
       <c r="E21">
-        <v>0.8673717856413896</v>
+        <v>0.6110093415514805</v>
       </c>
       <c r="F21">
         <v>30</v>
@@ -1592,28 +1592,28 @@
         <v>35</v>
       </c>
       <c r="J21">
-        <v>0.8383838383838383</v>
+        <v>0.8212765957446808</v>
       </c>
       <c r="K21">
-        <v>0.8686868686868687</v>
+        <v>0.7957446808510639</v>
       </c>
       <c r="L21">
-        <v>0.8682432432432432</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M21">
-        <v>0.847972972972973</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="N21">
-        <v>0.8682432432432432</v>
+        <v>0.8589743589743589</v>
       </c>
       <c r="O21">
-        <v>0.8583060333060333</v>
+        <v>0.8313693398799782</v>
       </c>
       <c r="P21">
-        <v>0.01271946549380881</v>
+        <v>0.0260482800074879</v>
       </c>
       <c r="Q21">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1621,16 +1621,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>939.7815648078919</v>
+        <v>695.3509555339813</v>
       </c>
       <c r="C22">
-        <v>30.57515336925603</v>
+        <v>17.8230321065717</v>
       </c>
       <c r="D22">
-        <v>9.064073467254639</v>
+        <v>9.251225090026855</v>
       </c>
       <c r="E22">
-        <v>0.4357053331546497</v>
+        <v>0.1543927244313818</v>
       </c>
       <c r="F22">
         <v>30</v>
@@ -1645,28 +1645,28 @@
         <v>36</v>
       </c>
       <c r="J22">
-        <v>0.8417508417508418</v>
+        <v>0.8212765957446808</v>
       </c>
       <c r="K22">
-        <v>0.8787878787878788</v>
+        <v>0.8</v>
       </c>
       <c r="L22">
-        <v>0.8682432432432432</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M22">
-        <v>0.8547297297297297</v>
+        <v>0.8127659574468085</v>
       </c>
       <c r="N22">
-        <v>0.8682432432432432</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O22">
-        <v>0.8623509873509873</v>
+        <v>0.8305146390252773</v>
       </c>
       <c r="P22">
-        <v>0.0128223112236802</v>
+        <v>0.02460232698404185</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1674,16 +1674,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>354.610577249527</v>
+        <v>264.8096826553345</v>
       </c>
       <c r="C23">
-        <v>10.38964514518066</v>
+        <v>7.85036294666071</v>
       </c>
       <c r="D23">
-        <v>7.905244588851929</v>
+        <v>7.770651197433471</v>
       </c>
       <c r="E23">
-        <v>0.4352450660722691</v>
+        <v>0.5118129740387306</v>
       </c>
       <c r="F23">
         <v>30</v>
@@ -1698,28 +1698,28 @@
         <v>37</v>
       </c>
       <c r="J23">
-        <v>0.8383838383838383</v>
+        <v>0.8425531914893617</v>
       </c>
       <c r="K23">
-        <v>0.8653198653198653</v>
+        <v>0.7872340425531915</v>
       </c>
       <c r="L23">
-        <v>0.8682432432432432</v>
+        <v>0.8595744680851064</v>
       </c>
       <c r="M23">
-        <v>0.847972972972973</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="N23">
-        <v>0.8682432432432432</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O23">
-        <v>0.8576326326326326</v>
+        <v>0.8322167666848518</v>
       </c>
       <c r="P23">
-        <v>0.01223183360106352</v>
+        <v>0.02688928450855228</v>
       </c>
       <c r="Q23">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1727,16 +1727,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>690.3180953502655</v>
+        <v>521.6976674079895</v>
       </c>
       <c r="C24">
-        <v>15.97915286520009</v>
+        <v>16.92341634488529</v>
       </c>
       <c r="D24">
-        <v>8.649898529052734</v>
+        <v>8.982001399993896</v>
       </c>
       <c r="E24">
-        <v>0.5153112233071498</v>
+        <v>0.1473352272916815</v>
       </c>
       <c r="F24">
         <v>30</v>
@@ -1751,28 +1751,28 @@
         <v>38</v>
       </c>
       <c r="J24">
-        <v>0.835016835016835</v>
+        <v>0.8382978723404255</v>
       </c>
       <c r="K24">
-        <v>0.8653198653198653</v>
+        <v>0.8</v>
       </c>
       <c r="L24">
-        <v>0.8682432432432432</v>
+        <v>0.8680851063829788</v>
       </c>
       <c r="M24">
-        <v>0.8445945945945946</v>
+        <v>0.8127659574468085</v>
       </c>
       <c r="N24">
-        <v>0.8716216216216216</v>
+        <v>0.8376068376068376</v>
       </c>
       <c r="O24">
-        <v>0.8569592319592321</v>
+        <v>0.83135115475541</v>
       </c>
       <c r="P24">
-        <v>0.01446767301397896</v>
+        <v>0.02351628422526605</v>
       </c>
       <c r="Q24">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1780,16 +1780,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1378.941379785538</v>
+        <v>1052.105046796799</v>
       </c>
       <c r="C25">
-        <v>39.78093660172509</v>
+        <v>30.78556927766398</v>
       </c>
       <c r="D25">
-        <v>9.357282876968384</v>
+        <v>9.253694772720337</v>
       </c>
       <c r="E25">
-        <v>0.2551467909733394</v>
+        <v>0.8147686189491606</v>
       </c>
       <c r="F25">
         <v>30</v>
@@ -1804,28 +1804,28 @@
         <v>39</v>
       </c>
       <c r="J25">
-        <v>0.8316498316498316</v>
+        <v>0.8340425531914893</v>
       </c>
       <c r="K25">
-        <v>0.8821548821548821</v>
+        <v>0.7914893617021277</v>
       </c>
       <c r="L25">
-        <v>0.8716216216216216</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M25">
-        <v>0.8547297297297297</v>
+        <v>0.8212765957446808</v>
       </c>
       <c r="N25">
-        <v>0.8648648648648649</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="O25">
-        <v>0.861004186004186</v>
+        <v>0.8313584288052374</v>
       </c>
       <c r="P25">
-        <v>0.01718158112116474</v>
+        <v>0.02437902330277207</v>
       </c>
       <c r="Q25">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1833,16 +1833,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>467.475831413269</v>
+        <v>355.5068373680115</v>
       </c>
       <c r="C26">
-        <v>18.31076503881954</v>
+        <v>6.747793308116449</v>
       </c>
       <c r="D26">
-        <v>8.720931577682496</v>
+        <v>8.485740423202515</v>
       </c>
       <c r="E26">
-        <v>0.1645285381023373</v>
+        <v>0.6035042847411959</v>
       </c>
       <c r="F26">
         <v>30</v>
@@ -1857,28 +1857,28 @@
         <v>40</v>
       </c>
       <c r="J26">
-        <v>0.835016835016835</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="K26">
-        <v>0.8552188552188552</v>
+        <v>0.8</v>
       </c>
       <c r="L26">
-        <v>0.8682432432432432</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M26">
-        <v>0.8547297297297297</v>
+        <v>0.825531914893617</v>
       </c>
       <c r="N26">
-        <v>0.875</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O26">
-        <v>0.8576417326417326</v>
+        <v>0.8322167666848518</v>
       </c>
       <c r="P26">
-        <v>0.01371085381161898</v>
+        <v>0.02374206183253689</v>
       </c>
       <c r="Q26">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1886,16 +1886,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>903.4715523719788</v>
+        <v>693.3658379077912</v>
       </c>
       <c r="C27">
-        <v>31.08110379396814</v>
+        <v>17.67863735076952</v>
       </c>
       <c r="D27">
-        <v>8.273106288909911</v>
+        <v>8.194056463241576</v>
       </c>
       <c r="E27">
-        <v>1.241276927579072</v>
+        <v>1.22271455683834</v>
       </c>
       <c r="F27">
         <v>30</v>
@@ -1910,28 +1910,28 @@
         <v>41</v>
       </c>
       <c r="J27">
-        <v>0.8282828282828283</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="K27">
-        <v>0.8754208754208754</v>
+        <v>0.8042553191489362</v>
       </c>
       <c r="L27">
-        <v>0.8648648648648649</v>
+        <v>0.8638297872340426</v>
       </c>
       <c r="M27">
-        <v>0.8513513513513513</v>
+        <v>0.8170212765957446</v>
       </c>
       <c r="N27">
-        <v>0.875</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O27">
-        <v>0.858983983983984</v>
+        <v>0.8313657028550645</v>
       </c>
       <c r="P27">
-        <v>0.01767533293242242</v>
+        <v>0.02343051053794231</v>
       </c>
       <c r="Q27">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1939,16 +1939,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1237.832046413422</v>
+        <v>930.9119723796845</v>
       </c>
       <c r="C28">
-        <v>187.7473157858151</v>
+        <v>124.8908186181419</v>
       </c>
       <c r="D28">
-        <v>2.665664291381836</v>
+        <v>2.555298233032226</v>
       </c>
       <c r="E28">
-        <v>1.71288041221839</v>
+        <v>1.667855269010148</v>
       </c>
       <c r="F28">
         <v>30</v>
@@ -1963,28 +1963,28 @@
         <v>42</v>
       </c>
       <c r="J28">
-        <v>0.8383838383838383</v>
+        <v>0.8297872340425532</v>
       </c>
       <c r="K28">
-        <v>0.8686868686868687</v>
+        <v>0.8085106382978723</v>
       </c>
       <c r="L28">
-        <v>0.8716216216216216</v>
+        <v>0.8595744680851064</v>
       </c>
       <c r="M28">
-        <v>0.8581081081081081</v>
+        <v>0.8085106382978723</v>
       </c>
       <c r="N28">
-        <v>0.8682432432432432</v>
+        <v>0.8547008547008547</v>
       </c>
       <c r="O28">
-        <v>0.861008736008736</v>
+        <v>0.8322167666848518</v>
       </c>
       <c r="P28">
-        <v>0.01220020321253987</v>
+        <v>0.02183502560051974</v>
       </c>
       <c r="Q28">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>